<commit_message>
Final mods to plot and fixes prior to launch
</commit_message>
<xml_diff>
--- a/public/data/templates/stomata-SR_author_year.xlsx
+++ b/public/data/templates/stomata-SR_author_year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daphnia/Dropbox/paleo-CO2 website files/proxy descriptions/3- stomatal frequency proxies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daphnia/Dropbox/proxy descriptions and data templates/3- stomatal frequency proxies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B6CA771-83AC-4142-8F72-531335AFD0C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F415A2-581D-6E4D-BEB8-1CA5B14ACE7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="460" windowWidth="28400" windowHeight="13680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="460" windowWidth="23820" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stomatal ratio" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="88">
   <si>
     <t>Laurus nobilis</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -212,12 +212,6 @@
     <t>person who entered data</t>
   </si>
   <si>
-    <t>date of data entry</t>
-  </si>
-  <si>
-    <t>Citation</t>
-  </si>
-  <si>
     <t>doi</t>
   </si>
   <si>
@@ -258,14 +252,6 @@
   </si>
   <si>
     <t>How was age determined?</t>
-  </si>
-  <si>
-    <t>Latitude, present-day (decimal degrees)</t>
-  </si>
-  <si>
-    <t>Longitude, 
-present-day
-(decimal degrees)</t>
   </si>
   <si>
     <t>Number of stomatal counts per leaf sample</t>
@@ -369,20 +355,41 @@
     <t>CO2_uncertainty_pos_ppm</t>
   </si>
   <si>
-    <t>CO2_uncertainty__neg_ppm</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>example data in first two rows: please delete before submitting spreadsheet with new data to database</t>
+    <t>CO2_uncertainty_neg_ppm</t>
+  </si>
+  <si>
+    <t>Reference of the data product</t>
+  </si>
+  <si>
+    <t>Modern Latitude (decimal degree, south negative)</t>
+  </si>
+  <si>
+    <t>Modern Longitude (decimal degree, west negative)</t>
+  </si>
+  <si>
+    <t>margret.stein@gmail.com</t>
+  </si>
+  <si>
+    <t>email of individual entering the data</t>
+  </si>
+  <si>
+    <t>example data in first row: please delete before submitting spreadsheet with new data to database</t>
+  </si>
+  <si>
+    <t>Paleo Latitude (decimal degree, south negative)</t>
+  </si>
+  <si>
+    <t>Paleo Longitude (decimal degree, west negative)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -468,8 +475,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -495,12 +517,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -513,7 +544,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -536,7 +567,13 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -820,11 +857,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY10"/>
+  <dimension ref="A3:BA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -852,711 +889,746 @@
     <col min="26" max="26" width="12.1640625" style="4" customWidth="1"/>
     <col min="27" max="27" width="10.6640625" style="4" customWidth="1"/>
     <col min="28" max="28" width="11.6640625" style="4" customWidth="1"/>
-    <col min="29" max="29" width="11.1640625" style="4" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" style="4" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" style="4"/>
-    <col min="32" max="32" width="10.83203125" style="4" customWidth="1"/>
-    <col min="33" max="33" width="11" style="4" customWidth="1"/>
-    <col min="34" max="41" width="8.83203125" style="4"/>
-    <col min="42" max="42" width="16" style="4" customWidth="1"/>
-    <col min="43" max="43" width="13" style="4" customWidth="1"/>
+    <col min="29" max="31" width="11.1640625" style="4" customWidth="1"/>
+    <col min="32" max="32" width="10.33203125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="8.83203125" style="4"/>
+    <col min="34" max="34" width="10.83203125" style="4" customWidth="1"/>
+    <col min="35" max="35" width="11" style="4" customWidth="1"/>
+    <col min="36" max="43" width="8.83203125" style="4"/>
     <col min="44" max="44" width="16" style="4" customWidth="1"/>
-    <col min="45" max="46" width="8.83203125" style="4"/>
-    <col min="47" max="48" width="13" style="4" customWidth="1"/>
-    <col min="49" max="49" width="12.33203125" style="4" customWidth="1"/>
-    <col min="50" max="50" width="16.83203125" style="4" customWidth="1"/>
-    <col min="51" max="51" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="16384" width="8.83203125" style="4"/>
+    <col min="45" max="45" width="13" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16" style="4" customWidth="1"/>
+    <col min="47" max="48" width="8.83203125" style="4"/>
+    <col min="49" max="50" width="13" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.33203125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="16.83203125" style="4" customWidth="1"/>
+    <col min="53" max="53" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="5" customFormat="1" ht="66" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="3" spans="1:53" s="5" customFormat="1" ht="66" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="H3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" s="5" customFormat="1" ht="24" customHeight="1">
+      <c r="A4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+    </row>
+    <row r="5" spans="1:53" s="7" customFormat="1">
+      <c r="A5" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="B5" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="C5">
+        <v>2019</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" ref="D5:D7" si="0">N5</f>
+        <v>10.1016/j.palaeo.2018.01.039</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E7" si="1">V5*1000</f>
+        <v>19000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F7" si="2">(W5-V5)*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G7" si="3">(V5-X5)*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" ref="H5:H7" si="4">AU5</f>
+        <v>491</v>
+      </c>
+      <c r="I5">
+        <f>AX5-AU5</f>
+        <v>110</v>
+      </c>
+      <c r="J5">
+        <f>AU5-AW5</f>
+        <v>110</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="N5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="7">
+        <v>19</v>
+      </c>
+      <c r="W5" s="7">
+        <v>21</v>
+      </c>
+      <c r="X5" s="7">
+        <v>17</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>9</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>7</v>
+      </c>
+      <c r="AG5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM5" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="AN5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AU5" s="7">
+        <v>491</v>
+      </c>
+      <c r="AV5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>381</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>601</v>
+      </c>
+      <c r="AY5" s="7">
+        <v>110</v>
+      </c>
+      <c r="AZ5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>30</v>
+      <c r="BA5" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:51" s="7" customFormat="1">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2">
+    <row r="6" spans="1:53">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6">
         <v>2019</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D5" si="0">N2</f>
-        <v>10.1016/j.palaeo.2018.01.039</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E5" si="1">V2*1000</f>
-        <v>19000</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F5" si="2">(W2-V2)*1000</f>
-        <v>2000</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G5" si="3">(V2-X2)*1000</f>
-        <v>2000</v>
-      </c>
-      <c r="H2" s="11">
-        <f t="shared" ref="H2:H5" si="4">AS2</f>
-        <v>491</v>
-      </c>
-      <c r="I2">
-        <f>AV2-AS2</f>
-        <v>110</v>
-      </c>
-      <c r="J2">
-        <f>AS2-AU2</f>
-        <v>110</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="9">
-        <v>43435</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" s="7">
-        <v>19</v>
-      </c>
-      <c r="W2" s="7">
-        <v>21</v>
-      </c>
-      <c r="X2" s="7">
-        <v>17</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA2" s="7">
-        <v>9</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD2" s="7">
-        <v>7</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK2" s="7">
-        <v>11.7</v>
-      </c>
-      <c r="AL2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AR2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS2" s="7">
-        <v>491</v>
-      </c>
-      <c r="AT2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AU2" s="7">
-        <v>381</v>
-      </c>
-      <c r="AV2" s="7">
-        <v>601</v>
-      </c>
-      <c r="AW2" s="7">
-        <v>110</v>
-      </c>
-      <c r="AX2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AY2" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" s="7" customFormat="1">
-      <c r="A3" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3" s="11"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="L3" s="9"/>
-      <c r="N3" s="3"/>
-      <c r="AQ3" s="4"/>
-      <c r="AY3" s="12"/>
-    </row>
-    <row r="4" spans="1:51">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4">
-        <v>2019</v>
-      </c>
-      <c r="D4" t="str">
+      <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>10.1016/j.palaeo.2018.01.039</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>22500</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="G4">
+      <c r="G6">
         <f t="shared" si="3"/>
         <v>1000</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H6" s="11">
         <f t="shared" si="4"/>
         <v>485</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I5" si="5">AV4-AS4</f>
+      <c r="I6">
+        <f t="shared" ref="I6:I7" si="5">AX6-AU6</f>
         <v>169</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J5" si="6">AS4-AU4</f>
+      <c r="J6">
+        <f t="shared" ref="J6:J7" si="6">AU6-AW6</f>
         <v>169</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="6">
-        <v>43435</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="L6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="T4" s="7" t="s">
+      <c r="Q6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="T6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V6" s="4">
         <v>22.5</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W6" s="4">
         <v>23.5</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X6" s="4">
         <v>21.5</v>
       </c>
-      <c r="Y4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z4" s="4" t="s">
+      <c r="Y6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA6" s="4">
         <v>9</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB6" s="4">
         <v>-45</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC6" s="4">
         <v>167</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF6" s="4">
         <v>7</v>
       </c>
-      <c r="AE4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AG6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AI6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK4" s="4">
+      <c r="AJ6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM6" s="4">
         <v>12.2</v>
       </c>
-      <c r="AL4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP4" s="7" t="s">
+      <c r="AN6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AQ4" s="7" t="s">
+      <c r="AS6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AR4" s="7" t="s">
+      <c r="AT6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AS4" s="7">
+      <c r="AU6" s="7">
         <v>485</v>
       </c>
-      <c r="AT4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AU4" s="7">
+      <c r="AV6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW6" s="7">
         <v>316</v>
       </c>
-      <c r="AV4" s="7">
+      <c r="AX6" s="7">
         <v>654</v>
       </c>
-      <c r="AW4" s="7">
+      <c r="AY6" s="7">
         <v>169</v>
       </c>
-      <c r="AX4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AY4" s="12" t="s">
-        <v>79</v>
+      <c r="AZ6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="BA6" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5">
+    <row r="7" spans="1:53">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7">
         <v>2019</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>10.1016/j.palaeo.2018.01.039</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>23200</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <f t="shared" si="2"/>
         <v>199.99999999999929</v>
       </c>
-      <c r="G5">
+      <c r="G7">
         <f t="shared" si="3"/>
         <v>199.99999999999929</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H7" s="11">
         <f t="shared" si="4"/>
         <v>732</v>
       </c>
-      <c r="I5">
+      <c r="I7">
         <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="J5">
+      <c r="J7">
         <f t="shared" si="6"/>
         <v>47</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="6">
-        <v>43435</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="3" t="s">
+      <c r="L7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="T5" s="7" t="s">
+      <c r="Q7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="T7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="U7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V7" s="4">
         <v>23.2</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W7" s="4">
         <v>23.4</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X7" s="4">
         <v>23</v>
       </c>
-      <c r="Y5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z5" s="4" t="s">
+      <c r="Y7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AA7" s="4">
         <v>3</v>
       </c>
-      <c r="AB5" s="8">
+      <c r="AB7" s="8">
         <v>-45.516666000000001</v>
       </c>
-      <c r="AC5" s="8">
+      <c r="AC7" s="8">
         <v>170.21665999999999</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AD7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF7" s="4">
         <v>7</v>
       </c>
-      <c r="AE5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AI7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK5" s="4">
+      <c r="AJ7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM7" s="4">
         <v>7.5</v>
       </c>
-      <c r="AL5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP5" s="7" t="s">
+      <c r="AN7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AQ5" s="7" t="s">
+      <c r="AS7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AR5" s="7" t="s">
+      <c r="AT7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AS5" s="7">
+      <c r="AU7" s="7">
         <v>732</v>
       </c>
-      <c r="AT5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AU5" s="7">
+      <c r="AV7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW7" s="7">
         <v>685</v>
       </c>
-      <c r="AV5" s="7">
+      <c r="AX7" s="7">
         <v>779</v>
       </c>
-      <c r="AW5" s="7">
+      <c r="AY7" s="7">
         <v>47</v>
       </c>
-      <c r="AX5" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AY5" s="12" t="s">
-        <v>79</v>
+      <c r="AZ7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="BA7" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6" s="11"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-    </row>
-    <row r="7" spans="1:51">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7" s="11"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8"/>
-    </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:53">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -1567,8 +1639,12 @@
       <c r="H8" s="11"/>
       <c r="I8"/>
       <c r="J8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:53">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -1579,8 +1655,12 @@
       <c r="H9" s="11"/>
       <c r="I9"/>
       <c r="J9"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:53">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -1592,12 +1672,36 @@
       <c r="I10"/>
       <c r="J10"/>
     </row>
+    <row r="11" spans="1:53">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11" s="11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:53">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12" s="11"/>
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="N4" r:id="rId2" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="N5" r:id="rId3" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N5" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N6" r:id="rId2" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N7" r:id="rId3" tooltip="Persistent link using digital object identifier" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>

</xml_diff>